<commit_message>
consolidated python notebook exercises and readme
</commit_message>
<xml_diff>
--- a/data/dataset_metadata.xlsx
+++ b/data/dataset_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alicia.brown/repos/connect/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D08FB7E-94B2-3146-A3D6-F371327C6059}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746FA1FD-99E1-A54B-A5C4-2563D93036D8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
-    <t>9abs-ubh5</t>
-  </si>
-  <si>
     <t>Arizona Places Median Household Income</t>
   </si>
   <si>
@@ -64,16 +61,19 @@
     <t>dataset_id</t>
   </si>
   <si>
-    <t>kyb6-5pf6</t>
-  </si>
-  <si>
     <t>Business</t>
   </si>
   <si>
     <t>income</t>
   </si>
   <si>
-    <t>7erx-nkcf</t>
+    <t>nump-7qcy</t>
+  </si>
+  <si>
+    <t>ebv5-4bfy</t>
+  </si>
+  <si>
+    <t>cfvy-xet3</t>
   </si>
 </sst>
 </file>
@@ -447,8 +447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -461,68 +461,68 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
         <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
       <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -530,23 +530,23 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
         <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{94AB4BA0-F978-E24F-B5CC-6DE3B25D4704}"/>
-    <hyperlink ref="A3" r:id="rId2" display="https://alicia.data.socrata.com/d/kyb6-5pf6" xr:uid="{CCA64A60-A27D-184A-BFCE-179F27C81277}"/>
-    <hyperlink ref="F3" r:id="rId3" xr:uid="{0A27E6E4-7E22-CC4E-9037-278AC9445B64}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{0A27E6E4-7E22-CC4E-9037-278AC9445B64}"/>
+    <hyperlink ref="A4" r:id="rId3" display="https://macondointernal.demo.socrata.com/d/cfvy-xet3" xr:uid="{A3D772E5-82FA-6440-A59E-C4910AF546CF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>